<commit_message>
initial sorting code, to be tested
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a72c8867ec6d2d80/Documents/GitHub/v1funnel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABDACC1048B3291F53885BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{212E8DF5-2A81-4FBF-966F-A9FF313982AB}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="11_F25DC773A252ABDACC1048B3291F53885BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C729F68C-F61C-4E5C-85AF-67A55371616F}"/>
   <bookViews>
-    <workbookView xWindow="-19298" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Arduino</t>
   </si>
@@ -103,6 +103,33 @@
   </si>
   <si>
     <t>Windmill motor</t>
+  </si>
+  <si>
+    <t>TCSLED</t>
+  </si>
+  <si>
+    <t>LEDC Channels</t>
+  </si>
+  <si>
+    <t>left motor a</t>
+  </si>
+  <si>
+    <t>right motor a</t>
+  </si>
+  <si>
+    <t>left motor b</t>
+  </si>
+  <si>
+    <t>right motor b</t>
+  </si>
+  <si>
+    <t>servo deposit</t>
+  </si>
+  <si>
+    <t>servo sort</t>
+  </si>
+  <si>
+    <t>windmill</t>
   </si>
 </sst>
 </file>
@@ -125,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +162,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -163,6 +196,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -445,50 +481,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AK5"/>
+  <dimension ref="B2:AK10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="1.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.06640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="1.73046875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>4</v>
       </c>
@@ -501,10 +539,10 @@
       <c r="E4" s="1">
         <v>7</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>15</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="5">
         <v>16</v>
       </c>
       <c r="H4" s="1">
@@ -513,7 +551,7 @@
       <c r="I4" s="1">
         <v>18</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="5">
         <v>8</v>
       </c>
       <c r="K4" s="1">
@@ -528,49 +566,49 @@
       <c r="N4" s="1">
         <v>10</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="5">
         <v>11</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="5">
         <v>12</v>
       </c>
       <c r="Q4" s="1">
         <v>13</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="5">
         <v>14</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="5">
         <v>47</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4" s="5">
         <v>48</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4" s="5">
         <v>21</v>
       </c>
       <c r="V4" s="1">
         <v>45</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4" s="5">
         <v>0</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="5">
         <v>35</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Y4" s="5">
         <v>36</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="Z4" s="5">
         <v>37</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AA4" s="5">
         <v>38</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="5">
         <v>39</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AC4" s="5">
         <v>40</v>
       </c>
       <c r="AD4" s="1">
@@ -598,14 +636,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F5" s="1" t="s">
+    <row r="5" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -614,43 +652,46 @@
       <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="R5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="T5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AB5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AC5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AD5" s="4" t="s">
@@ -667,6 +708,60 @@
       </c>
       <c r="AI5" s="4" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started IR code, need to test IR detector
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a72c8867ec6d2d80/Documents/GitHub/v1funnel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="11_F25DC773A252ABDACC1048B3291F53885BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69E922FB-D852-4EBB-BE46-FD54D018C057}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="11_F25DC773A252ABDACC1048B3291F53885BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C5AC28D-5C88-4119-89E1-7ED51A390D19}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Arduino</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>windmill</t>
+  </si>
+  <si>
+    <t>IR</t>
   </si>
 </sst>
 </file>
@@ -484,49 +487,49 @@
   <dimension ref="B2:AK10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="2.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.1328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="3.265625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.1328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="2.1328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>4</v>
       </c>
@@ -614,7 +617,7 @@
       <c r="AD4" s="1">
         <v>41</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AE4" s="5">
         <v>42</v>
       </c>
       <c r="AF4" s="1">
@@ -636,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
@@ -658,6 +661,9 @@
       <c r="P5" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="Q5" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="R5" s="5" t="s">
         <v>26</v>
       </c>
@@ -697,7 +703,7 @@
       <c r="AD5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AE5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="AF5" s="4" t="s">
@@ -710,12 +716,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0</v>
       </c>
@@ -741,7 +747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
milestone 4 done, just need return code
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a72c8867ec6d2d80/Documents/GitHub/v1funnel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="11_F25DC773A252ABDACC1048B3291F53885BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C5AC28D-5C88-4119-89E1-7ED51A390D19}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="11_F25DC773A252ABDACC1048B3291F53885BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B12BEE1E-5F4F-45BC-AD61-7DA59154E7DD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Arduino</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>IR</t>
+  </si>
+  <si>
+    <t>Win B</t>
   </si>
 </sst>
 </file>
@@ -486,50 +489,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="5" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.265625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.3984375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.1328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.1328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.59765625" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:37" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1">
         <v>4</v>
       </c>
@@ -575,7 +582,7 @@
       <c r="P4" s="5">
         <v>12</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="5">
         <v>13</v>
       </c>
       <c r="R4" s="5">
@@ -614,16 +621,16 @@
       <c r="AC4" s="5">
         <v>40</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AD4" s="5">
         <v>41</v>
       </c>
       <c r="AE4" s="5">
         <v>42</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AF4" s="5">
         <v>44</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AG4" s="5">
         <v>43</v>
       </c>
       <c r="AH4" s="1">
@@ -639,13 +646,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:37" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="J5" s="5" t="s">
         <v>25</v>
       </c>
@@ -661,7 +671,7 @@
       <c r="P5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="R5" s="5" t="s">
@@ -700,28 +710,28 @@
       <c r="AC5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AD5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="AE5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AF5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AG5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="AI5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:37" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:37" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>0</v>
       </c>
@@ -747,7 +757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:37" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -768,6 +778,9 @@
       </c>
       <c r="H10" t="s">
         <v>33</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>